<commit_message>
Updated Chrome Desired Capabilities
</commit_message>
<xml_diff>
--- a/SeleniumTestAutomationRunner(STAR)/DB.xlsx
+++ b/SeleniumTestAutomationRunner(STAR)/DB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="133">
   <si>
     <t>TCID</t>
   </si>
@@ -404,6 +404,18 @@
   </si>
   <si>
     <t>Trivandrum</t>
+  </si>
+  <si>
+    <t>TCID_0</t>
+  </si>
+  <si>
+    <t>http://google.com</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>SearchImpl.openSearchEngine</t>
   </si>
 </sst>
 </file>
@@ -825,7 +837,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -870,82 +882,99 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="7" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B4" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="6" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B5" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="7" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1717,7 +1746,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1772,190 +1801,176 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="11">
+      <c r="A2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="14">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="C2" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="11">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J4" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="13"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="7" t="s">
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B5" s="14">
         <v>1</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J5" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="10"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="6" t="s">
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H6" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J6" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="14">
-        <v>1</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="K6" s="10"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="7" t="s">
         <v>104</v>
       </c>
       <c r="B7" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>66</v>
@@ -1967,7 +1982,7 @@
         <v>66</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="K7" s="10"/>
     </row>
@@ -1976,43 +1991,77 @@
         <v>104</v>
       </c>
       <c r="B8" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>66</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>66</v>
       </c>
       <c r="J8" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="14">
+        <v>3</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="K8" s="10"/>
+      <c r="K9" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C7" r:id="rId5"/>
+    <hyperlink ref="C8" r:id="rId6"/>
+    <hyperlink ref="C9" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhanced object identification logic
</commit_message>
<xml_diff>
--- a/SeleniumTestAutomationRunner(STAR)/DB.xlsx
+++ b/SeleniumTestAutomationRunner(STAR)/DB.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="136">
   <si>
     <t>TCID</t>
   </si>
@@ -416,6 +416,15 @@
   </si>
   <si>
     <t>SearchImpl.openSearchEngine</t>
+  </si>
+  <si>
+    <t>MAIN_FLOW_1</t>
+  </si>
+  <si>
+    <t>Regression:Custom</t>
+  </si>
+  <si>
+    <t>200</t>
   </si>
 </sst>
 </file>
@@ -837,14 +846,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -975,6 +984,21 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1414,7 +1438,7 @@
         <v>85</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1746,13 +1770,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -1821,7 +1845,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="6" t="s">
-        <v>46</v>
+        <v>133</v>
       </c>
       <c r="B3" s="11">
         <v>1</v>
@@ -1833,7 +1857,7 @@
         <v>128</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>65</v>
@@ -1859,151 +1883,151 @@
         <v>46</v>
       </c>
       <c r="B4" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="11">
+        <v>2</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H5" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="13"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="7" t="s">
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B6" s="14">
         <v>1</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H6" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="6" t="s">
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B7" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H7" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J7" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="K6" s="13"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" s="14">
-        <v>1</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="K7" s="10"/>
+      <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="7" t="s">
         <v>104</v>
       </c>
       <c r="B8" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>66</v>
@@ -2015,7 +2039,7 @@
         <v>66</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="K8" s="10"/>
     </row>
@@ -2024,44 +2048,78 @@
         <v>104</v>
       </c>
       <c r="B9" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>66</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>66</v>
       </c>
       <c r="J9" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="14">
+        <v>3</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J10" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="K9" s="10"/>
+      <c r="K10" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C6" r:id="rId4"/>
-    <hyperlink ref="C7" r:id="rId5"/>
-    <hyperlink ref="C8" r:id="rId6"/>
-    <hyperlink ref="C9" r:id="rId7"/>
+    <hyperlink ref="C6" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
+    <hyperlink ref="C7" r:id="rId4"/>
+    <hyperlink ref="C8" r:id="rId5"/>
+    <hyperlink ref="C9" r:id="rId6"/>
+    <hyperlink ref="C10" r:id="rId7"/>
     <hyperlink ref="C2" r:id="rId8"/>
+    <hyperlink ref="C3" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>